<commit_message>
HE cases running but need adjustments
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_HE01.xlsx
+++ b/integration_testing/projects/bestest_HE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2314,7 +2314,7 @@
     <t>|HE100 - Base-case Building and Mechanical Systems|</t>
   </si>
   <si>
-    <t>BESTEST Heating 06712b (1.12.1 run)</t>
+    <t>BESTEST Heating 06712d (hvac wtih oa)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixes Fan for Heating cases issue #19
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_HE01.xlsx
+++ b/integration_testing/projects/bestest_HE01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-20" windowWidth="25600" windowHeight="28260" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2260,9 +2260,6 @@
     <t>bestest_he_reporting</t>
   </si>
   <si>
-    <t>BESTEST Heating 060906 (updated outputs tab)</t>
-  </si>
-  <si>
     <t>bestest_he_reporting.total_furnace_load</t>
   </si>
   <si>
@@ -2270,6 +2267,9 @@
   </si>
   <si>
     <t>bestest_he_reporting.average_fuel_consumption</t>
+  </si>
+  <si>
+    <t>BESTEST Heating 061027b (fixing case 170)</t>
   </si>
 </sst>
 </file>
@@ -6015,8 +6015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6187,7 +6187,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -8287,7 +8287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
@@ -8742,7 +8742,7 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="45" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>730</v>
@@ -8771,7 +8771,7 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="45" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="45" t="s">
@@ -8798,7 +8798,7 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="45" t="s">

</xml_diff>